<commit_message>
feat: (WIP) memory for my_mod_csr
</commit_message>
<xml_diff>
--- a/FPGA/synth/ram/doc/Excel/timing_diagram_ram_sp_wf.xlsx
+++ b/FPGA/synth/ram/doc/Excel/timing_diagram_ram_sp_wf.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motchy\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motchy\Documents\GitHub\code-fractions\FPGA\synth\ram\doc\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66263BBC-0658-4D2E-BEB2-57747F74D0B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A352F507-EDCC-4511-8347-90DA6A49A603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="14540" xr2:uid="{D9A37A3E-2F6F-469C-A47D-D0E2A71B6F48}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="25">
   <si>
     <t>i_data</t>
     <phoneticPr fontId="1"/>
@@ -124,6 +124,14 @@
   </si>
   <si>
     <t>example @ read latency = 2 cycles</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>i_byte_en</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>'1</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -280,13 +288,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
@@ -301,29 +306,32 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="centerContinuous" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,10 +656,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9DE142AE-25F5-48BD-ADD7-F8A509CB2382}">
-  <dimension ref="A1:AA17"/>
+  <dimension ref="A1:AA19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AE19" sqref="AE19"/>
+      <selection activeCell="AE12" sqref="AE12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -667,7 +675,7 @@
       </c>
     </row>
     <row r="3" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="19" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
@@ -700,39 +708,14 @@
       <c r="AA3" s="5"/>
     </row>
     <row r="4" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="13"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="6"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
+      <c r="A4" s="19"/>
     </row>
     <row r="5" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="13"/>
+      <c r="A5" s="19"/>
       <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="7"/>
+      <c r="C5" s="6"/>
       <c r="D5" s="5"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
@@ -759,14 +742,14 @@
       <c r="AA5" s="3"/>
     </row>
     <row r="6" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="13"/>
+      <c r="A6" s="19"/>
     </row>
     <row r="7" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A7" s="13"/>
+      <c r="A7" s="19"/>
       <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="1">
@@ -781,14 +764,14 @@
         <v>2</v>
       </c>
       <c r="I7" s="2"/>
-      <c r="J7" s="17">
+      <c r="J7" s="14">
         <v>3</v>
       </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="17">
+      <c r="K7" s="15"/>
+      <c r="L7" s="14">
         <v>4</v>
       </c>
-      <c r="M7" s="18"/>
+      <c r="M7" s="15"/>
       <c r="N7" s="1">
         <v>5</v>
       </c>
@@ -801,14 +784,14 @@
         <v>7</v>
       </c>
       <c r="S7" s="2"/>
-      <c r="T7" s="17">
+      <c r="T7" s="14">
         <v>0</v>
       </c>
-      <c r="U7" s="18"/>
-      <c r="V7" s="17">
+      <c r="U7" s="15"/>
+      <c r="V7" s="14">
         <v>1</v>
       </c>
-      <c r="W7" s="18"/>
+      <c r="W7" s="15"/>
       <c r="X7" s="1">
         <v>2</v>
       </c>
@@ -819,241 +802,241 @@
       <c r="AA7" s="2"/>
     </row>
     <row r="8" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="13"/>
+      <c r="A8" s="19"/>
     </row>
     <row r="9" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="13"/>
+      <c r="A9" s="19"/>
       <c r="B9" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="9"/>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
-      <c r="O9" s="10"/>
-      <c r="P9" s="20"/>
-      <c r="Q9" s="19"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="19"/>
-      <c r="T9" s="9"/>
-      <c r="U9" s="10"/>
-      <c r="V9" s="10"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="10"/>
-      <c r="Y9" s="10"/>
-      <c r="Z9" s="10"/>
-      <c r="AA9" s="10"/>
+      <c r="C9" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="16"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="9"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9"/>
+      <c r="P9" s="17"/>
+      <c r="Q9" s="16"/>
+      <c r="R9" s="16"/>
+      <c r="S9" s="16"/>
+      <c r="T9" s="8"/>
+      <c r="U9" s="9"/>
+      <c r="V9" s="9"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="9"/>
+      <c r="Y9" s="9"/>
+      <c r="Z9" s="9"/>
+      <c r="AA9" s="9"/>
     </row>
     <row r="10" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="13"/>
+      <c r="A10" s="19"/>
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="13"/>
+      <c r="A11" s="19"/>
       <c r="B11" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="15" t="s">
+      <c r="C11" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E11" s="16"/>
-      <c r="F11" s="15" t="s">
+      <c r="E11" s="13"/>
+      <c r="F11" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G11" s="16"/>
-      <c r="H11" s="15" t="s">
+      <c r="G11" s="13"/>
+      <c r="H11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I11" s="16"/>
-      <c r="J11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="K11" s="12"/>
-      <c r="L11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="M11" s="12"/>
-      <c r="N11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="O11" s="12"/>
-      <c r="P11" s="15" t="s">
+      <c r="I11" s="13"/>
+      <c r="J11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M11" s="11"/>
+      <c r="N11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="O11" s="11"/>
+      <c r="P11" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="Q11" s="16"/>
-      <c r="R11" s="15" t="s">
+      <c r="Q11" s="13"/>
+      <c r="R11" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="S11" s="16"/>
-      <c r="T11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="U11" s="12"/>
-      <c r="V11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="W11" s="12"/>
-      <c r="X11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="Y11" s="12"/>
-      <c r="Z11" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA11" s="12"/>
+      <c r="S11" s="13"/>
+      <c r="T11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="U11" s="11"/>
+      <c r="V11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="W11" s="11"/>
+      <c r="X11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y11" s="11"/>
+      <c r="Z11" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="AA11" s="11"/>
     </row>
     <row r="12" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" s="13"/>
+      <c r="A12" s="19"/>
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A13" s="13"/>
+      <c r="A13" s="19"/>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="I13" s="2"/>
+      <c r="J13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="K13" s="2"/>
+      <c r="L13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="O13" s="2"/>
+      <c r="P13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q13" s="2"/>
+      <c r="R13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="S13" s="2"/>
+      <c r="T13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="U13" s="2"/>
+      <c r="V13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="W13" s="2"/>
+      <c r="X13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="Y13" s="2"/>
+      <c r="Z13" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="AA13" s="2"/>
+    </row>
+    <row r="14" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="19"/>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="19"/>
+      <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="C13" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D13" s="1">
-        <f>D17</f>
+      <c r="C15" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="1">
+        <f>D19</f>
         <v>0</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="15" t="str">
-        <f>F17</f>
+      <c r="E15" s="2"/>
+      <c r="F15" s="12" t="str">
+        <f>F19</f>
         <v>data0</v>
       </c>
-      <c r="G13" s="16"/>
-      <c r="H13" s="15" t="str">
-        <f t="shared" ref="H13:Q13" si="0">H17</f>
+      <c r="G15" s="13"/>
+      <c r="H15" s="12" t="str">
+        <f t="shared" ref="H15" si="0">H19</f>
         <v>data1</v>
       </c>
-      <c r="I13" s="16"/>
-      <c r="J13" s="15" t="str">
-        <f t="shared" ref="J13:Q13" si="1">J17</f>
+      <c r="I15" s="13"/>
+      <c r="J15" s="12" t="str">
+        <f t="shared" ref="J15" si="1">J19</f>
         <v>data2</v>
       </c>
-      <c r="K13" s="16"/>
-      <c r="L13" s="1" t="str">
-        <f t="shared" ref="L13:Q13" si="2">L17</f>
+      <c r="K15" s="13"/>
+      <c r="L15" s="1" t="str">
+        <f t="shared" ref="L15" si="2">L19</f>
         <v>data2</v>
       </c>
-      <c r="M13" s="2"/>
-      <c r="N13" s="17" t="str">
-        <f t="shared" ref="N13:Q13" si="3">N17</f>
+      <c r="M15" s="2"/>
+      <c r="N15" s="14" t="str">
+        <f t="shared" ref="N15" si="3">N19</f>
         <v>data[3]</v>
       </c>
-      <c r="O13" s="18"/>
-      <c r="P13" s="17" t="str">
-        <f t="shared" ref="P13:Q13" si="4">P17</f>
+      <c r="O15" s="15"/>
+      <c r="P15" s="14" t="str">
+        <f t="shared" ref="P15" si="4">P19</f>
         <v>data[4]</v>
       </c>
-      <c r="Q13" s="18"/>
-      <c r="R13" s="15" t="str">
-        <f>R17</f>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="12" t="str">
+        <f>R19</f>
         <v>data10</v>
       </c>
-      <c r="S13" s="16"/>
-      <c r="T13" s="15" t="str">
-        <f>T17</f>
+      <c r="S15" s="13"/>
+      <c r="T15" s="12" t="str">
+        <f>T19</f>
         <v>data11</v>
       </c>
-      <c r="U13" s="16"/>
-      <c r="V13" s="1" t="str">
-        <f t="shared" ref="V13:AA13" si="5">V17</f>
+      <c r="U15" s="13"/>
+      <c r="V15" s="1" t="str">
+        <f t="shared" ref="V15" si="5">V19</f>
         <v>data11</v>
       </c>
-      <c r="W13" s="2"/>
-      <c r="X13" s="17" t="str">
-        <f t="shared" ref="X13:AA13" si="6">X17</f>
+      <c r="W15" s="2"/>
+      <c r="X15" s="14" t="str">
+        <f t="shared" ref="X15" si="6">X19</f>
         <v>data[0]</v>
       </c>
-      <c r="Y13" s="18"/>
-      <c r="Z13" s="17" t="str">
-        <f t="shared" ref="Z13:AA13" si="7">Z17</f>
+      <c r="Y15" s="15"/>
+      <c r="Z15" s="14" t="str">
+        <f t="shared" ref="Z15" si="7">Z19</f>
         <v>data[1]</v>
       </c>
-      <c r="AA13" s="18"/>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A15" s="14" t="s">
+      <c r="AA15" s="15"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C15" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="1">
-        <v>0</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="2"/>
-      <c r="H15" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I15" s="2"/>
-      <c r="J15" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="M15" s="2"/>
-      <c r="N15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="O15" s="2"/>
-      <c r="P15" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="S15" s="2"/>
-      <c r="T15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="U15" s="2"/>
-      <c r="V15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="W15" s="2"/>
-      <c r="X15" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="Y15" s="2"/>
-      <c r="Z15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AA15" s="2"/>
-    </row>
-    <row r="16" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" s="14"/>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="14"/>
-      <c r="B17" t="s">
-        <v>9</v>
-      </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>5</v>
       </c>
       <c r="D17" s="1">
@@ -1073,15 +1056,15 @@
       </c>
       <c r="K17" s="2"/>
       <c r="L17" s="1" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="M17" s="2"/>
       <c r="N17" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="O17" s="2"/>
       <c r="P17" s="1" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" s="1" t="s">
@@ -1093,22 +1076,82 @@
       </c>
       <c r="U17" s="2"/>
       <c r="V17" s="1" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="W17" s="2"/>
       <c r="X17" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="Y17" s="2"/>
       <c r="Z17" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="AA17" s="2"/>
+    </row>
+    <row r="18" spans="1:27" ht="6" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="18"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="18"/>
+      <c r="B19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0</v>
+      </c>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I19" s="2"/>
+      <c r="J19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K19" s="2"/>
+      <c r="L19" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O19" s="2"/>
+      <c r="P19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q19" s="2"/>
+      <c r="R19" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="S19" s="2"/>
+      <c r="T19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="U19" s="2"/>
+      <c r="V19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="W19" s="2"/>
+      <c r="X19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Y19" s="2"/>
+      <c r="Z19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA17" s="2"/>
+      <c r="AA19" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A3:A13"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="A3:A15"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>